<commit_message>
06/07/2025 Final Version With All Edited
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Tracks &amp; Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B70259-E5C2-4F20-9E4B-34B5C44A1630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC40972C-D636-40FC-9EF1-C7CA7B33FC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2235,6 +2235,91 @@
     <t>Converting integer to currency format</t>
   </si>
   <si>
+    <t>Simple Fun #1 Seats in Theater</t>
+  </si>
+  <si>
+    <t>Reverse List Order</t>
+  </si>
+  <si>
+    <t>Hello, Name or World!</t>
+  </si>
+  <si>
+    <t>Find the Remainder</t>
+  </si>
+  <si>
+    <t>Find The Position</t>
+  </si>
+  <si>
+    <t>Find the Difference in Age between Oldest and Youngest Family Members</t>
+  </si>
+  <si>
+    <t>Multiply Word in String</t>
+  </si>
+  <si>
+    <t>Check if a triangle is an equable triangle!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (713)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Needs Review</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (66)</t>
+    </r>
+  </si>
+  <si>
+    <t>Factorial(2)</t>
+  </si>
+  <si>
+    <t>Get the Middle Character</t>
+  </si>
+  <si>
+    <t>FIXME Hello</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -2245,7 +2330,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CodeWars(582)</t>
+      <t>CodeWars(583)</t>
     </r>
     <r>
       <rPr>
@@ -2295,55 +2380,29 @@
       </rPr>
       <t>leetCode(26)</t>
     </r>
-  </si>
-  <si>
-    <t>Simple Fun #1 Seats in Theater</t>
-  </si>
-  <si>
-    <t>Reverse List Order</t>
-  </si>
-  <si>
-    <t>Hello, Name or World!</t>
-  </si>
-  <si>
-    <t>Find the Remainder</t>
-  </si>
-  <si>
-    <t>Find The Position</t>
-  </si>
-  <si>
-    <t>Find the Difference in Age between Oldest and Youngest Family Members</t>
-  </si>
-  <si>
-    <t>Multiply Word in String</t>
-  </si>
-  <si>
-    <t>Check if a triangle is an equable triangle!</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
         <i/>
-        <sz val="14"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>All</t>
+      <t xml:space="preserve"> - </t>
     </r>
     <r>
       <rPr>
         <b/>
         <i/>
-        <sz val="14"/>
-        <color rgb="FF00B050"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (713)</t>
+      <t>Exponent (1)</t>
     </r>
   </si>
   <si>
@@ -2369,43 +2428,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> (221 Yes) (442 No) (80 Hint)</t>
+      <t xml:space="preserve"> (212 Yes) (420 No) (81 Hint)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Needs Review</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (66)</t>
-    </r>
-  </si>
-  <si>
-    <t>Factorial(2)</t>
-  </si>
-  <si>
-    <t>Get the Middle Character</t>
-  </si>
-  <si>
-    <t>FIXME Hello</t>
   </si>
 </sst>
 </file>
@@ -3807,8 +3831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A703" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A716" sqref="A716"/>
+    <sheetView tabSelected="1" topLeftCell="A698" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C717" sqref="C717"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5595,7 +5619,7 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="105" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>23</v>
@@ -9528,7 +9552,7 @@
     </row>
     <row r="249" spans="1:7">
       <c r="A249" s="13" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B249" s="4" t="s">
         <v>23</v>
@@ -10057,7 +10081,7 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" s="132" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B272" s="4" t="s">
         <v>23</v>
@@ -10609,7 +10633,7 @@
     </row>
     <row r="296" spans="1:7">
       <c r="A296" s="53" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B296" s="4" t="s">
         <v>23</v>
@@ -11437,7 +11461,7 @@
     </row>
     <row r="332" spans="1:7">
       <c r="A332" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B332" s="4" t="s">
         <v>23</v>
@@ -11552,7 +11576,7 @@
     </row>
     <row r="337" spans="1:7">
       <c r="A337" s="4" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B337" s="4" t="s">
         <v>23</v>
@@ -11713,7 +11737,7 @@
     </row>
     <row r="344" spans="1:7">
       <c r="A344" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B344" s="4" t="s">
         <v>23</v>
@@ -17261,7 +17285,7 @@
     </row>
     <row r="585" spans="1:7">
       <c r="A585" s="37" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B585" s="4" t="s">
         <v>23</v>
@@ -19127,7 +19151,7 @@
     </row>
     <row r="666" spans="1:7">
       <c r="A666" s="104" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B666" s="4" t="s">
         <v>23</v>
@@ -20208,7 +20232,7 @@
     </row>
     <row r="713" spans="1:7">
       <c r="A713" s="58" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B713" s="4" t="s">
         <v>23</v>
@@ -20231,7 +20255,7 @@
     </row>
     <row r="714" spans="1:7">
       <c r="A714" s="55" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B714" s="4" t="s">
         <v>23</v>
@@ -20272,22 +20296,22 @@
     </row>
     <row r="721" spans="1:1" ht="18.75">
       <c r="A721" s="79" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="722" spans="1:1" ht="18.75">
       <c r="A722" s="79" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
     </row>
     <row r="723" spans="1:1" ht="18.75">
       <c r="A723" s="79" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" s="5" t="s">
-        <v>736</v>
+        <v>749</v>
       </c>
     </row>
     <row r="743" spans="1:6" ht="15.75">

</xml_diff>

<commit_message>
Review 10 Problem Solving 1/11/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5655E0-78ED-4E5B-A37E-810BB81666DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924D24F6-6083-43A1-929E-C512C1107BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3169,7 +3169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3212,6 +3212,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3241,7 +3247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="46" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3685,6 +3691,9 @@
     <xf numFmtId="0" fontId="45" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3982,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4482,7 +4491,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="151" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -4500,7 +4509,7 @@
       <c r="F22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4523,7 +4532,7 @@
       <c r="F23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4546,7 +4555,7 @@
       <c r="F24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G24" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4569,7 +4578,7 @@
       <c r="F25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4592,7 +4601,7 @@
       <c r="F26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4615,7 +4624,7 @@
       <c r="F27" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4638,7 +4647,7 @@
       <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G28" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4661,7 +4670,7 @@
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4684,7 +4693,7 @@
       <c r="F30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4707,7 +4716,7 @@
       <c r="F31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Solved 10 Problems 1/12/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924D24F6-6083-43A1-929E-C512C1107BEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C090E40B-2CD7-4226-9A87-ADFB1F3547B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3991,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4739,7 +4739,7 @@
       <c r="F32" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4762,7 +4762,7 @@
       <c r="F33" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4785,7 +4785,7 @@
       <c r="F34" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G34" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4808,7 +4808,7 @@
       <c r="F35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
       <c r="F36" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G36" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4854,7 +4854,7 @@
       <c r="F37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G37" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4877,7 +4877,7 @@
       <c r="F38" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G38" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4900,7 +4900,7 @@
       <c r="F39" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4923,7 +4923,7 @@
       <c r="F40" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="G40" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4946,7 +4946,7 @@
       <c r="F41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 20 Problems 1/18/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C090E40B-2CD7-4226-9A87-ADFB1F3547B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5198D8D-171C-4752-BF55-71C92D893A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2547,7 +2547,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="71">
+  <fonts count="72">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3168,6 +3168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -3247,7 +3256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="46" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3694,6 +3703,9 @@
     <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3991,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4969,7 +4981,7 @@
       <c r="F42" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G42" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -4992,7 +5004,7 @@
       <c r="F43" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="G43" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5015,7 +5027,7 @@
       <c r="F44" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5038,7 +5050,7 @@
       <c r="F45" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G45" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5061,7 +5073,7 @@
       <c r="F46" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5084,7 +5096,7 @@
       <c r="F47" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5107,7 +5119,7 @@
       <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G48" s="20" t="s">
+      <c r="G48" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5130,7 +5142,7 @@
       <c r="F49" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G49" s="20" t="s">
+      <c r="G49" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5153,7 +5165,7 @@
       <c r="F50" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G50" s="20" t="s">
+      <c r="G50" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5176,7 +5188,7 @@
       <c r="F51" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5199,7 +5211,7 @@
       <c r="F52" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G52" s="20" t="s">
+      <c r="G52" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5222,7 +5234,7 @@
       <c r="F53" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G53" s="20" t="s">
+      <c r="G53" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5245,7 +5257,7 @@
       <c r="F54" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G54" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5268,7 +5280,7 @@
       <c r="F55" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5291,7 +5303,7 @@
       <c r="F56" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5314,7 +5326,7 @@
       <c r="F57" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="20" t="s">
+      <c r="G57" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5325,7 +5337,7 @@
       <c r="B58" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D58" s="12">
@@ -5337,7 +5349,7 @@
       <c r="F58" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G58" s="20" t="s">
+      <c r="G58" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5348,7 +5360,7 @@
       <c r="B59" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D59" s="12">
@@ -5360,7 +5372,7 @@
       <c r="F59" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G59" s="20" t="s">
+      <c r="G59" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5371,7 +5383,7 @@
       <c r="B60" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="12">
@@ -5383,7 +5395,7 @@
       <c r="F60" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="20" t="s">
+      <c r="G60" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5394,7 +5406,7 @@
       <c r="B61" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D61" s="12">
@@ -5406,7 +5418,7 @@
       <c r="F61" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="20" t="s">
+      <c r="G61" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reivewed 20 Problems 1/18/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177DC5BA-5A71-460F-8A08-BEA7EFF4FEB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E53A4D-67C9-43B2-B43F-A57FCCEA720C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5441,7 +5441,7 @@
       <c r="F62" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G62" s="20" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reviewed 10 problems 1/26/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E53A4D-67C9-43B2-B43F-A57FCCEA720C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB644CB-766F-4F95-B717-7D47D644CF97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5441,7 +5441,7 @@
       <c r="F62" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G62" s="20" t="s">
+      <c r="G62" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5464,7 +5464,7 @@
       <c r="F63" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G63" s="20" t="s">
+      <c r="G63" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       <c r="F64" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G64" s="20" t="s">
+      <c r="G64" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5510,7 +5510,7 @@
       <c r="F65" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G65" s="20" t="s">
+      <c r="G65" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5521,7 +5521,7 @@
       <c r="B66" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D66" s="12">
@@ -5533,7 +5533,7 @@
       <c r="F66" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5544,7 +5544,7 @@
       <c r="B67" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="152" t="s">
         <v>13</v>
       </c>
       <c r="D67" s="12">
@@ -5579,7 +5579,7 @@
       <c r="F68" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G68" s="20" t="s">
+      <c r="G68" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5602,7 +5602,7 @@
       <c r="F69" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G69" s="20" t="s">
+      <c r="G69" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
       <c r="F70" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G70" s="20" t="s">
+      <c r="G70" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5648,7 +5648,7 @@
       <c r="F71" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G71" s="20" t="s">
+      <c r="G71" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 10 Problems 1/28/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E702EEE-B682-46EA-BCCB-D2B67AF6BF6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123EF941-5D2B-4D40-8F75-65542676DE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5901,7 +5901,7 @@
       <c r="F82" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G82" s="20" t="s">
+      <c r="G82" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5924,7 +5924,7 @@
       <c r="F83" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G83" s="20" t="s">
+      <c r="G83" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       <c r="F84" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G84" s="20" t="s">
+      <c r="G84" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5970,7 +5970,7 @@
       <c r="F85" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G85" s="20" t="s">
+      <c r="G85" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6016,7 +6016,7 @@
       <c r="F87" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G87" s="20" t="s">
+      <c r="G87" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6039,7 +6039,7 @@
       <c r="F88" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G88" s="20" t="s">
+      <c r="G88" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6062,7 +6062,7 @@
       <c r="F89" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G89" s="20" t="s">
+      <c r="G89" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6085,7 +6085,7 @@
       <c r="F90" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G90" s="20" t="s">
+      <c r="G90" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6108,7 +6108,7 @@
       <c r="F91" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G91" s="20" t="s">
+      <c r="G91" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 20 Problem 2/4/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123EF941-5D2B-4D40-8F75-65542676DE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA34F7-CBB1-4BF8-89AB-C58599AE0C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6131,7 +6131,7 @@
       <c r="F92" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G92" s="20" t="s">
+      <c r="G92" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6154,7 +6154,7 @@
       <c r="F93" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G93" s="20" t="s">
+      <c r="G93" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       <c r="F94" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G94" s="20" t="s">
+      <c r="G94" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6200,7 +6200,7 @@
       <c r="F95" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G95" s="20" t="s">
+      <c r="G95" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6223,7 +6223,7 @@
       <c r="F96" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G96" s="20" t="s">
+      <c r="G96" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
       <c r="F98" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G98" s="20" t="s">
+      <c r="G98" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6315,7 +6315,7 @@
       <c r="F100" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G100" s="20" t="s">
+      <c r="G100" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6338,7 +6338,7 @@
       <c r="F101" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G101" s="20" t="s">
+      <c r="G101" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6361,7 +6361,7 @@
       <c r="F102" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G102" s="20" t="s">
+      <c r="G102" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6384,7 +6384,7 @@
       <c r="F103" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G103" s="20" t="s">
+      <c r="G103" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6407,7 +6407,7 @@
       <c r="F104" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G104" s="20" t="s">
+      <c r="G104" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6430,7 +6430,7 @@
       <c r="F105" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G105" s="20" t="s">
+      <c r="G105" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6453,7 +6453,7 @@
       <c r="F106" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G106" s="20" t="s">
+      <c r="G106" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6476,7 +6476,7 @@
       <c r="F107" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G107" s="20" t="s">
+      <c r="G107" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6499,7 +6499,7 @@
       <c r="F108" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G108" s="20" t="s">
+      <c r="G108" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6522,7 +6522,7 @@
       <c r="F109" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G109" s="20" t="s">
+      <c r="G109" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6545,7 +6545,7 @@
       <c r="F110" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G110" s="20" t="s">
+      <c r="G110" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6568,7 +6568,7 @@
       <c r="F111" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G111" s="20" t="s">
+      <c r="G111" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 20 Problem 2/8/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA34F7-CBB1-4BF8-89AB-C58599AE0C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B668823-5C14-4A7B-94AA-726EEB8EB6F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6591,7 +6591,7 @@
       <c r="F112" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G112" s="20" t="s">
+      <c r="G112" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6614,7 +6614,7 @@
       <c r="F113" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G113" s="20" t="s">
+      <c r="G113" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6637,7 +6637,7 @@
       <c r="F114" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G114" s="20" t="s">
+      <c r="G114" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6660,7 +6660,7 @@
       <c r="F115" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G115" s="20" t="s">
+      <c r="G115" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6683,7 +6683,7 @@
       <c r="F116" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G116" s="20" t="s">
+      <c r="G116" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6706,7 +6706,7 @@
       <c r="F117" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G117" s="20" t="s">
+      <c r="G117" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6729,7 +6729,7 @@
       <c r="F118" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G118" s="20" t="s">
+      <c r="G118" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6752,7 +6752,7 @@
       <c r="F119" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G119" s="20" t="s">
+      <c r="G119" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6775,7 +6775,7 @@
       <c r="F120" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G120" s="20" t="s">
+      <c r="G120" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6798,7 +6798,7 @@
       <c r="F121" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G121" s="20" t="s">
+      <c r="G121" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6821,7 +6821,7 @@
       <c r="F122" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G122" s="20" t="s">
+      <c r="G122" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6844,7 +6844,7 @@
       <c r="F123" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="20" t="s">
+      <c r="G123" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6867,7 +6867,7 @@
       <c r="F124" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G124" s="20" t="s">
+      <c r="G124" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6890,7 +6890,7 @@
       <c r="F125" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G125" s="20" t="s">
+      <c r="G125" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6913,7 +6913,7 @@
       <c r="F126" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G126" s="20" t="s">
+      <c r="G126" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6936,7 +6936,7 @@
       <c r="F127" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G127" s="20" t="s">
+      <c r="G127" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6959,7 +6959,7 @@
       <c r="F128" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G128" s="20" t="s">
+      <c r="G128" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6982,7 +6982,7 @@
       <c r="F129" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G129" s="20" t="s">
+      <c r="G129" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7005,7 +7005,7 @@
       <c r="F130" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G130" s="20" t="s">
+      <c r="G130" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7028,7 +7028,7 @@
       <c r="F131" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G131" s="20" t="s">
+      <c r="G131" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 10 Problems 2/9/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B668823-5C14-4A7B-94AA-726EEB8EB6F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F62A83-CAD4-4473-B918-DE4D957C8111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7051,7 +7051,7 @@
       <c r="F132" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G132" s="20" t="s">
+      <c r="G132" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7074,7 +7074,7 @@
       <c r="F133" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G133" s="20" t="s">
+      <c r="G133" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7097,7 +7097,7 @@
       <c r="F134" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G134" s="20" t="s">
+      <c r="G134" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7120,7 +7120,7 @@
       <c r="F135" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G135" s="20" t="s">
+      <c r="G135" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7143,7 +7143,7 @@
       <c r="F136" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G136" s="20" t="s">
+      <c r="G136" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7166,7 +7166,7 @@
       <c r="F137" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G137" s="20" t="s">
+      <c r="G137" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7189,7 +7189,7 @@
       <c r="F138" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G138" s="20" t="s">
+      <c r="G138" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7212,7 +7212,7 @@
       <c r="F139" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G139" s="20" t="s">
+      <c r="G139" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7235,7 +7235,7 @@
       <c r="F140" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G140" s="20" t="s">
+      <c r="G140" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7258,7 +7258,7 @@
       <c r="F141" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G141" s="20" t="s">
+      <c r="G141" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 10 Problems 2/10/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F62A83-CAD4-4473-B918-DE4D957C8111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E2F3DD-3194-4329-B80A-AF7A988434E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7281,7 +7281,7 @@
       <c r="F142" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G142" s="20" t="s">
+      <c r="G142" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7304,7 +7304,7 @@
       <c r="F143" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G143" s="20" t="s">
+      <c r="G143" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7327,7 +7327,7 @@
       <c r="F144" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G144" s="20" t="s">
+      <c r="G144" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7350,7 +7350,7 @@
       <c r="F145" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G145" s="20" t="s">
+      <c r="G145" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7373,7 +7373,7 @@
       <c r="F146" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G146" s="20" t="s">
+      <c r="G146" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7396,7 +7396,7 @@
       <c r="F147" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G147" s="20" t="s">
+      <c r="G147" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7419,7 +7419,7 @@
       <c r="F148" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G148" s="20" t="s">
+      <c r="G148" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7442,7 +7442,7 @@
       <c r="F149" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G149" s="20" t="s">
+      <c r="G149" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7465,7 +7465,7 @@
       <c r="F150" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G150" s="20" t="s">
+      <c r="G150" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7488,7 +7488,7 @@
       <c r="F151" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G151" s="20" t="s">
+      <c r="G151" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7511,7 +7511,7 @@
       <c r="F152" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G152" s="20" t="s">
+      <c r="G152" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7534,7 +7534,7 @@
       <c r="F153" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G153" s="20" t="s">
+      <c r="G153" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       <c r="F154" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G154" s="20" t="s">
+      <c r="G154" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7580,7 +7580,7 @@
       <c r="F155" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G155" s="20" t="s">
+      <c r="G155" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       <c r="F156" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G156" s="20" t="s">
+      <c r="G156" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7626,7 +7626,7 @@
       <c r="F157" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G157" s="20" t="s">
+      <c r="G157" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7649,7 +7649,7 @@
       <c r="F158" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G158" s="20" t="s">
+      <c r="G158" s="50" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7672,7 +7672,7 @@
       <c r="F159" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="20" t="s">
+      <c r="G159" s="50" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Review 10 Problems 2/21/2026
</commit_message>
<xml_diff>
--- a/Problem Solving History.xlsx
+++ b/Problem Solving History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Career\Courses\Web Development\Problem Solving\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E2F3DD-3194-4329-B80A-AF7A988434E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C18A8B6-3CAC-422A-9D96-604ACC59EF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4003,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFC1C95-6620-4666-A840-FB4F0938EA8B}">
   <dimension ref="A1:H782"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D154" sqref="D154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7511,7 +7511,7 @@
       <c r="F152" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G152" s="50" t="s">
+      <c r="G152" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7534,7 +7534,7 @@
       <c r="F153" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G153" s="50" t="s">
+      <c r="G153" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7557,7 +7557,7 @@
       <c r="F154" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G154" s="50" t="s">
+      <c r="G154" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7580,7 +7580,7 @@
       <c r="F155" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G155" s="50" t="s">
+      <c r="G155" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7603,7 +7603,7 @@
       <c r="F156" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G156" s="50" t="s">
+      <c r="G156" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7626,7 +7626,7 @@
       <c r="F157" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G157" s="50" t="s">
+      <c r="G157" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7649,7 +7649,7 @@
       <c r="F158" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G158" s="50" t="s">
+      <c r="G158" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7672,7 +7672,7 @@
       <c r="F159" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="50" t="s">
+      <c r="G159" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7695,7 +7695,7 @@
       <c r="F160" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G160" s="50" t="s">
+      <c r="G160" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7718,7 +7718,7 @@
       <c r="F161" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G161" s="50" t="s">
+      <c r="G161" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -7741,7 +7741,7 @@
       <c r="F162" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G162" s="50" t="s">
+      <c r="G162" s="11" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>